<commit_message>
commit with excel file
</commit_message>
<xml_diff>
--- a/SA_Info.xlsx
+++ b/SA_Info.xlsx
@@ -32,10 +32,10 @@
       <style:table-column-properties fo:break-before="auto" style:column-width="1.679cm"/>
     </style:style>
     <style:style style:name="co2" style:family="table-column">
-      <style:table-column-properties fo:break-before="auto" style:column-width="2.745cm"/>
+      <style:table-column-properties fo:break-before="auto" style:column-width="5.913cm"/>
     </style:style>
     <style:style style:name="co3" style:family="table-column">
-      <style:table-column-properties fo:break-before="auto" style:column-width="14.815cm"/>
+      <style:table-column-properties fo:break-before="auto" style:column-width="20.241cm"/>
     </style:style>
     <style:style style:name="ro1" style:family="table-row">
       <style:table-row-properties style:row-height="0.413cm" fo:break-before="auto" style:use-optimal-row-height="true"/>
@@ -46,6 +46,9 @@
     <style:style style:name="ro3" style:family="table-row">
       <style:table-row-properties style:row-height="0.497cm" fo:break-before="auto" style:use-optimal-row-height="true"/>
     </style:style>
+    <style:style style:name="ro4" style:family="table-row">
+      <style:table-row-properties style:row-height="0.542cm" fo:break-before="auto" style:use-optimal-row-height="true"/>
+    </style:style>
     <style:style style:name="ta1" style:family="table" style:master-page-name="PageStyle_5f_Login">
       <style:table-properties table:display="true" style:writing-mode="lr-tb"/>
     </style:style>
@@ -59,13 +62,13 @@
       <style:text-properties fo:color="#0000ff" style:text-outline="false" style:text-line-through-style="none" style:font-name="Arial" fo:font-size="10pt" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="normal" style:font-size-asian="10pt" style:font-style-asian="normal" style:font-weight-asian="normal" style:font-name-complex="Arial" style:font-size-complex="10pt" style:font-style-complex="normal" style:font-weight-complex="normal"/>
     </style:style>
     <style:style style:name="ce2" style:family="table-cell" style:parent-style-name="Default">
+      <style:text-properties fo:font-weight="bold" style:font-weight-asian="bold" style:font-weight-complex="bold"/>
+    </style:style>
+    <style:style style:name="ce3" style:family="table-cell" style:parent-style-name="Default">
       <style:text-properties style:use-window-font-color="true" style:text-outline="false" style:text-line-through-style="none" style:font-name="Liberation Serif" fo:font-size="10pt" fo:language="en" fo:country="US" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="normal" style:text-underline-mode="continuous" style:text-overline-mode="continuous" style:text-line-through-mode="continuous" style:font-name-asian="Liberation Serif" style:font-size-asian="10pt" style:language-asian="en" style:country-asian="US" style:font-style-asian="normal" style:font-weight-asian="normal" style:font-size-complex="5.65000009536743pt" style:language-complex="en" style:country-complex="US" style:font-style-complex="normal" style:font-weight-complex="normal" style:text-emphasize="none" style:font-relief="none" style:text-overline-style="none" style:text-overline-color="font-color"/>
     </style:style>
-    <style:style style:name="ce3" style:family="table-cell" style:parent-style-name="Default">
+    <style:style style:name="ce4" style:family="table-cell" style:parent-style-name="Default">
       <style:text-properties fo:color="#0f7003" style:text-outline="false" style:text-line-through-style="none" style:font-name="Menlo" fo:font-size="12pt" fo:language="en" fo:country="US" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="bold" style:text-underline-mode="continuous" style:text-overline-mode="continuous" style:text-line-through-mode="continuous" style:font-name-asian="Menlo" style:font-size-asian="12pt" style:language-asian="en" style:country-asian="US" style:font-style-asian="normal" style:font-weight-asian="bold" style:font-size-complex="6.80000019073486pt" style:language-complex="en" style:country-complex="US" style:font-style-complex="normal" style:font-weight-complex="bold" style:text-emphasize="none" style:font-relief="none" style:text-overline-style="none" style:text-overline-color="font-color"/>
-    </style:style>
-    <style:style style:name="ce4" style:family="table-cell" style:parent-style-name="Default">
-      <style:text-properties fo:color="#0f7003" style:font-name="Menlo" fo:font-size="12pt" fo:language="en" fo:country="US" fo:font-weight="bold" style:font-name-asian="Menlo" style:font-size-asian="12pt" style:language-asian="en" style:country-asian="US" style:font-weight-asian="bold" style:font-name-complex="Menlo" style:font-size-complex="6.80000019073486pt" style:language-complex="en" style:country-complex="US" style:font-weight-complex="bold"/>
     </style:style>
   </office:automatic-styles>
   <office:body>
@@ -104,44 +107,77 @@
       <table:table table:name="XPath" table:style-name="ta3" table:print="false">
         <office:forms form:automatic-focus="false" form:apply-design-mode="false"/>
         <table:table-column table:style-name="co2" table:default-cell-style-name="Default"/>
-        <table:table-column table:style-name="co3" table:default-cell-style-name="ce3"/>
+        <table:table-column table:style-name="co3" table:default-cell-style-name="ce4"/>
         <table:table-column table:style-name="co1" table:number-columns-repeated="1022" table:default-cell-style-name="Default"/>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell table:style-name="ce2" office:value-type="string">
+            <text:p>login page</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="Default"/>
+          <table:table-cell table:number-columns-repeated="1022"/>
+        </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string">
             <text:p>username</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1023"/>
+          <table:table-cell office:value-type="string">
+            <text:p>//INPUT[@type='text']"</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1022"/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string">
             <text:p>verify me </text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce4"/>
+          <table:table-cell office:value-type="string">
+            <text:p>/html/body/div[1]/div/div/div[2]/div/form/div[3]/button"</text:p>
+          </table:table-cell>
           <table:table-cell table:number-columns-repeated="1022"/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string">
             <text:p>password </text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1023"/>
+          <table:table-cell office:value-type="string">
+            <text:p>//INPUT[@type='password']"</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1022"/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string">
             <text:p>login button </text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1023"/>
+          <table:table-cell office:value-type="string">
+            <text:p>/html/body/div[1]/div/div/div[2]/div/form/div[4]/button[1]</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1022"/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string">
             <text:p>logout previous</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1023"/>
+          <table:table-cell office:value-type="string">
+            <text:p>/html/body/div[1]/div/div/div[2]/div[2]/div[2]/button</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1022"/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
-          <table:table-cell table:style-name="ce2" office:value-type="string">
+          <table:table-cell table:style-name="ce3" office:value-type="string">
             <text:p>Profile Menu</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1023"/>
+          <table:table-cell office:value-type="string">
+            <text:p>(//I[@class='fa fa-caret-down'])[2]</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1022"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro4">
+          <table:table-cell office:value-type="string">
+            <text:p>click on logout</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string">
+            <text:p>//SPAN[@class='node_modules-fk-cs-dropdown-dropdown_options'][text()='Logout']</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1022"/>
         </table:table-row>
       </table:table>
     </office:spreadsheet>
@@ -152,11 +188,11 @@
 <file path=meta.xml><?xml version="1.0" encoding="utf-8"?>
 <office:document-meta xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:grddl="http://www.w3.org/2003/g/data-view#" office:version="1.2">
   <office:meta>
-    <dc:date>2018-02-07T13:10:10</dc:date>
+    <dc:date>2018-02-08T12:29:36</dc:date>
     <meta:generator>OpenOffice.org/3.4$Unix OpenOffice.org_project/340m1$Build-9590</meta:generator>
-    <meta:editing-duration>PT4M57S</meta:editing-duration>
-    <meta:editing-cycles>3</meta:editing-cycles>
-    <meta:document-statistic meta:table-count="3" meta:cell-count="10" meta:object-count="0"/>
+    <meta:editing-duration>PT24M46S</meta:editing-duration>
+    <meta:editing-cycles>15</meta:editing-cycles>
+    <meta:document-statistic meta:table-count="3" meta:cell-count="19" meta:object-count="0"/>
   </office:meta>
 </office:document-meta>
 </file>
@@ -167,8 +203,8 @@
     <config:config-item-set config:name="ooo:view-settings">
       <config:config-item config:name="VisibleAreaTop" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaLeft" config:type="int">0</config:config-item>
-      <config:config-item config:name="VisibleAreaWidth" config:type="int">3345</config:config-item>
-      <config:config-item config:name="VisibleAreaHeight" config:type="int">838</config:config-item>
+      <config:config-item config:name="VisibleAreaWidth" config:type="int">26055</config:config-item>
+      <config:config-item config:name="VisibleAreaHeight" config:type="int">3924</config:config-item>
       <config:config-item-map-indexed config:name="Views">
         <config:config-item-map-entry>
           <config:config-item config:name="ViewId" config:type="string">view1</config:config-item>
@@ -206,8 +242,8 @@
               <config:config-item config:name="PageViewZoomValue" config:type="int">60</config:config-item>
             </config:config-item-map-entry>
             <config:config-item-map-entry config:name="XPath">
-              <config:config-item config:name="CursorPositionX" config:type="int">1</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">15</config:config-item>
+              <config:config-item config:name="CursorPositionX" config:type="int">0</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">19</config:config-item>
               <config:config-item config:name="HorizontalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="VerticalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="HorizontalSplitPosition" config:type="int">0</config:config-item>
@@ -343,68 +379,64 @@
       <number:number number:decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
       <style:map style:condition="value()&gt;=0" style:apply-style-name="N5109P0"/>
     </number:number-style>
-    <number:number-style style:name="N5110P0" style:volatile="true" number:language="en" number:country="IN">
-      <number:text> </number:text>
+    <number:number-style style:name="N5113P0" style:volatile="true" number:language="en" number:country="IN">
       <number:number number:decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
       <number:text> </number:text>
     </number:number-style>
-    <number:number-style style:name="N5110P1" style:volatile="true" number:language="en" number:country="IN">
+    <number:number-style style:name="N5113P1" style:volatile="true" number:language="en" number:country="IN">
       <number:text>-</number:text>
       <number:number number:decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
       <number:text> </number:text>
     </number:number-style>
-    <number:number-style style:name="N5110P2" style:volatile="true" number:language="en" number:country="IN">
+    <number:number-style style:name="N5113P2" style:volatile="true" number:language="en" number:country="IN">
       <number:text> - </number:text>
     </number:number-style>
-    <number:text-style style:name="N5110" number:language="en" number:country="IN">
-      <number:text> </number:text>
+    <number:text-style style:name="N5113" number:language="en" number:country="IN">
       <number:text-content/>
       <number:text> </number:text>
-      <style:map style:condition="value()&gt;0" style:apply-style-name="N5110P0"/>
-      <style:map style:condition="value()&lt;0" style:apply-style-name="N5110P1"/>
-      <style:map style:condition="value()=0" style:apply-style-name="N5110P2"/>
+      <style:map style:condition="value()&gt;0" style:apply-style-name="N5113P0"/>
+      <style:map style:condition="value()&lt;0" style:apply-style-name="N5113P1"/>
+      <style:map style:condition="value()=0" style:apply-style-name="N5113P2"/>
     </number:text-style>
-    <number:number-style style:name="N5111P0" style:volatile="true" number:language="en" number:country="IN">
+    <number:number-style style:name="N5117P0" style:volatile="true" number:language="en" number:country="IN">
+      <number:number number:decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
       <number:text> </number:text>
+    </number:number-style>
+    <number:number-style style:name="N5117P1" style:volatile="true" number:language="en" number:country="IN">
+      <number:text>-</number:text>
       <number:number number:decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
       <number:text> </number:text>
     </number:number-style>
-    <number:number-style style:name="N5111P1" style:volatile="true" number:language="en" number:country="IN">
-      <number:text>-</number:text>
-      <number:number number:decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:number-style>
-    <number:number-style style:name="N5111P2" style:volatile="true" number:language="en" number:country="IN">
+    <number:number-style style:name="N5117P2" style:volatile="true" number:language="en" number:country="IN">
       <number:text> -</number:text>
       <number:number number:decimal-places="0" number:min-integer-digits="0"/>
       <number:text> </number:text>
     </number:number-style>
-    <number:text-style style:name="N5111" number:language="en" number:country="IN">
-      <number:text> </number:text>
+    <number:text-style style:name="N5117" number:language="en" number:country="IN">
       <number:text-content/>
       <number:text> </number:text>
-      <style:map style:condition="value()&gt;0" style:apply-style-name="N5111P0"/>
-      <style:map style:condition="value()&lt;0" style:apply-style-name="N5111P1"/>
-      <style:map style:condition="value()=0" style:apply-style-name="N5111P2"/>
+      <style:map style:condition="value()&gt;0" style:apply-style-name="N5117P0"/>
+      <style:map style:condition="value()&lt;0" style:apply-style-name="N5117P1"/>
+      <style:map style:condition="value()=0" style:apply-style-name="N5117P2"/>
     </number:text-style>
-    <number:time-style style:name="N5112" number:language="en" number:country="IN">
+    <number:time-style style:name="N5118" number:language="en" number:country="IN">
       <number:minutes number:style="long"/>
       <number:text>:</number:text>
       <number:seconds number:style="long"/>
     </number:time-style>
-    <number:time-style style:name="N5113" number:language="en" number:country="IN" number:truncate-on-overflow="false">
+    <number:time-style style:name="N5119" number:language="en" number:country="IN" number:truncate-on-overflow="false">
       <number:hours/>
       <number:text>:</number:text>
       <number:minutes number:style="long"/>
       <number:text>:</number:text>
       <number:seconds number:style="long"/>
     </number:time-style>
-    <number:time-style style:name="N5114" number:language="en" number:country="IN">
+    <number:time-style style:name="N5120" number:language="en" number:country="IN">
       <number:minutes number:style="long"/>
       <number:text>:</number:text>
       <number:seconds number:style="long" number:decimal-places="1"/>
     </number:time-style>
-    <number:number-style style:name="N5115" number:language="en" number:country="IN">
+    <number:number-style style:name="N5121" number:language="en" number:country="IN">
       <number:scientific-number number:decimal-places="1" number:min-integer-digits="3" number:min-exponent-digits="1"/>
     </number:number-style>
     <style:style style:name="Default" style:family="table-cell">
@@ -500,9 +532,9 @@
         </style:region-left>
         <style:region-right>
           <text:p>
-            <text:date style:data-style-name="N2" text:date-value="2018-02-07">07/02/2018</text:date>
+            <text:date style:data-style-name="N2" text:date-value="2018-02-08">08/02/2018</text:date>
             , 
-            <text:time>13:10:10</text:time>
+            <text:time>12:29:36</text:time>
           </text:p>
         </style:region-right>
       </style:header>

</xml_diff>